<commit_message>
Updated model and tests
Updated model and testing
</commit_message>
<xml_diff>
--- a/M_OutputV1.xlsx
+++ b/M_OutputV1.xlsx
@@ -501,40 +501,40 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>1289.512385074049</v>
+        <v>1065.9912109375</v>
       </c>
       <c r="C4">
-        <v>1209.412897769362</v>
+        <v>1765.9912109375</v>
       </c>
       <c r="D4">
-        <v>1559.435686863959</v>
+        <v>1765.9912109375</v>
       </c>
       <c r="E4">
-        <v>1354.763845186206</v>
+        <v>1722.556936324731</v>
       </c>
       <c r="F4">
-        <v>1010.359581313401</v>
+        <v>1366.818344318289</v>
       </c>
       <c r="G4">
-        <v>668.3428142902052</v>
+        <v>1216.635531668583</v>
       </c>
       <c r="H4">
-        <v>619.6382072902966</v>
+        <v>1156.106598544197</v>
       </c>
       <c r="I4">
-        <v>648.4470932395986</v>
+        <v>1319.303949254877</v>
       </c>
       <c r="J4">
-        <v>790.0138481595834</v>
+        <v>1108.752176372667</v>
       </c>
       <c r="K4">
-        <v>783.460523458232</v>
+        <v>1280.174344915785</v>
       </c>
       <c r="L4">
-        <v>779.976789589013</v>
+        <v>1272.80688884724</v>
       </c>
       <c r="M4">
-        <v>778.1011715847945</v>
+        <v>1268.806893988051</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -703,16 +703,16 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>598.8321940104166</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>437.1866861979166</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>291.3770887586805</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>145.9438747829861</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -733,10 +733,10 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>169.4727456771422</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>430.9061684267506</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -744,19 +744,19 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1552.079274275585</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1274.032423231337</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1055.096605088976</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>285.3435940212673</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>66.27349853515625</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -768,16 +768,16 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>455.0533139694706</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>591.0131448400665</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>772.4486837814333</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>1371.918776554871</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -785,40 +785,40 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>663.2033770840765</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>862.204231576264</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>487.1439084968382</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>112.3658730150698</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>206.4625277806191</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>469.747638254256</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>731.4354739476157</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>997.5525851536704</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>869.0742594158232</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>657.0091349041045</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>316.8818995448789</v>
       </c>
     </row>
   </sheetData>
@@ -905,16 +905,16 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>145.48095703125</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>131.2286376953125</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>130.889892578125</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>131.3494873046875</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -946,19 +946,19 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>250.2421659398235</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>197.042236328125</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>692.7777099609375</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>197.1630859375</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>59.64614868164062</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -990,13 +990,13 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>337.5542907714831</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>337.3002319335916</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>101.1292857135628</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1011,13 +1011,13 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>115.6304931640625</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>190.8586120605469</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>306.114511823303</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1134,13 +1134,13 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>188.3030507523802</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>290.4815808328982</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>186.5844728707401</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1169,19 +1169,19 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>505.6147932994118</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>151.0664787451066</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>201.5950432681852</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>666.077880859375</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>200.1783308007934</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1189,7 +1189,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>221.112060546875</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1201,16 +1201,16 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>229.4028086451323</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>292.5390116373744</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>290.7642618815107</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>295.6856791178386</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1222,7 +1222,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>384.8016417102195</v>
       </c>
     </row>
   </sheetData>
@@ -1309,16 +1309,16 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1358.116021248546</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>755.0064595323779</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>148.2573275879334</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>148.2573275879334</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>193.7963971105556</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>326.051739475036</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>625.0428692568726</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>969.0747812288578</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1350,40 +1350,40 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>2376.26038288242</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1709.593716215753</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1114.40260835985</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>574.767056059503</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>90.68705931471136</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>224.4899601240531</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>658.5451358640626</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>677.1010557030895</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1217.10105570309</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1757.10105570309</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>1836.26038288242</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1394,37 +1394,37 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>135.1702880859375</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>315.3405761718739</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>540.5108642578094</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>810.6811523437469</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1122.311553955075</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1433.941955566403</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1688.369598388672</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1444.444444444444</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>970.5342610677083</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>496.6240776909721</v>
       </c>
     </row>
   </sheetData>
@@ -1511,16 +1511,16 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>542.7986055445515</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>546.07421875</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>133.4315948291401</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1552,19 +1552,19 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>535.6719970703125</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>485.6719970703125</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>435.6719970703125</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>81.61835338324022</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1617,16 +1617,16 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>426.5191650390625</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>426.5191650390625</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>446.9616699218749</v>
       </c>
     </row>
   </sheetData>
@@ -1734,19 +1734,19 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>215.3293301228396</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>146.9503804049782</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>332.2123664242629</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>382.2576799688724</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>432.2680444663206</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1769,25 +1769,25 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>249.4332890267256</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>482.2835286000105</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>20.61768871002995</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>87.95480797703362</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1795,28 +1795,28 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>150.189208984375</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>200.1892089843737</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>250.1892089843728</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>300.189208984375</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>346.2560017903646</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>346.2560017903646</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>282.697380913632</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>346.2560017903646</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1921,28 +1921,28 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1951,10 +1951,10 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1963,40 +1963,40 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>315.6280517578125</v>
+        <v>301.79443359375</v>
       </c>
       <c r="D5">
-        <v>395.7275390625</v>
+        <v>301.79443359375</v>
       </c>
       <c r="E5">
-        <v>45.70474996790296</v>
+        <v>301.79443359375</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>301.79443359375</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>391.3803100585938</v>
       </c>
       <c r="H5">
-        <v>213.7453217943979</v>
+        <v>391.3803100585938</v>
       </c>
       <c r="I5">
-        <v>208.2707913826852</v>
+        <v>391.3803100585938</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>391.3803100585938</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>557.1990966796875</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>557.1990966796875</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>557.1990966796875</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>557.1990966796875</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -2007,40 +2007,40 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -2049,40 +2049,40 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>317.572021484375</v>
+        <v>253.7078857421875</v>
       </c>
       <c r="D7">
-        <v>363.8427734375</v>
+        <v>253.7078857421875</v>
       </c>
       <c r="E7">
-        <v>384.307861328125</v>
+        <v>253.7078857421875</v>
       </c>
       <c r="F7">
-        <v>262.9963816702366</v>
+        <v>253.7078857421875</v>
       </c>
       <c r="G7">
-        <v>235.3967010427012</v>
+        <v>350.5338033040364</v>
       </c>
       <c r="H7">
-        <v>295.6663946043857</v>
+        <v>350.5338033040364</v>
       </c>
       <c r="I7">
-        <v>241.8674639191255</v>
+        <v>350.5338033040364</v>
       </c>
       <c r="J7">
-        <v>226.9921863299325</v>
+        <v>350.5338033040364</v>
       </c>
       <c r="K7">
-        <v>222.8792071212922</v>
+        <v>494.4839477539062</v>
       </c>
       <c r="L7">
-        <v>221.7419780599</v>
+        <v>494.4839477539062</v>
       </c>
       <c r="M7">
-        <v>221.427536903631</v>
+        <v>494.4839477539062</v>
       </c>
       <c r="N7">
-        <v>221.3405946647169</v>
+        <v>494.4839477539062</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -2093,40 +2093,40 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -2135,40 +2135,40 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>184.2086791992188</v>
+        <v>100.189208984375</v>
       </c>
       <c r="D9">
-        <v>164.697265625</v>
+        <v>100.189208984375</v>
       </c>
       <c r="E9">
-        <v>180.6289672851562</v>
+        <v>100.189208984375</v>
       </c>
       <c r="F9">
-        <v>150.0946044921875</v>
+        <v>100.189208984375</v>
       </c>
       <c r="G9">
-        <v>151.6720823154902</v>
+        <v>146.2560017903646</v>
       </c>
       <c r="H9">
-        <v>119.2316011052148</v>
+        <v>146.2560017903646</v>
       </c>
       <c r="I9">
-        <v>111.9118487467763</v>
+        <v>82.69738091362763</v>
       </c>
       <c r="J9">
-        <v>110.2602464095121</v>
+        <v>146.2560017903646</v>
       </c>
       <c r="K9">
-        <v>109.8875848566507</v>
+        <v>182.84912109375</v>
       </c>
       <c r="L9">
-        <v>109.8034988573471</v>
+        <v>182.84912109375</v>
       </c>
       <c r="M9">
-        <v>109.7845259978594</v>
+        <v>182.84912109375</v>
       </c>
       <c r="N9">
-        <v>109.7802450307529</v>
+        <v>182.84912109375</v>
       </c>
     </row>
   </sheetData>
@@ -2264,40 +2264,40 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="F4">
-        <v>106.1938468441367</v>
+        <v>400</v>
       </c>
       <c r="G4">
-        <v>24.2408047211357</v>
+        <v>300</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>48.53973126529024</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>82.75415938552746</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>182.7541593855275</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>82.75415938552744</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2306,40 +2306,40 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>607.1661368831992</v>
+        <v>444.93408203125</v>
       </c>
       <c r="D5">
-        <v>592.9138175472617</v>
+        <v>444.93408203125</v>
       </c>
       <c r="E5">
-        <v>592.5750724300742</v>
+        <v>444.93408203125</v>
       </c>
       <c r="F5">
-        <v>486.8408203125</v>
+        <v>444.93408203125</v>
       </c>
       <c r="G5">
-        <v>489.97802734375</v>
+        <v>554.6821412915192</v>
       </c>
       <c r="H5">
-        <v>419.8873297826998</v>
+        <v>519.1098549070936</v>
       </c>
       <c r="I5">
-        <v>391.5906790785564</v>
+        <v>577.1668739320045</v>
       </c>
       <c r="J5">
-        <v>374.8825904202108</v>
+        <v>607.403564453125</v>
       </c>
       <c r="K5">
-        <v>359.1308643102561</v>
+        <v>638.6974209605322</v>
       </c>
       <c r="L5">
-        <v>360.3496600123211</v>
+        <v>744.970703125</v>
       </c>
       <c r="M5">
-        <v>358.3347255753044</v>
+        <v>744.970703125</v>
       </c>
       <c r="N5">
-        <v>362.2859663632733</v>
+        <v>744.970703125</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -2350,40 +2350,40 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -2392,40 +2392,40 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>296.5686167776585</v>
+        <v>384.1156005859375</v>
       </c>
       <c r="D7">
-        <v>314.6086253225803</v>
+        <v>384.1156005859375</v>
       </c>
       <c r="E7">
-        <v>293.8894785940647</v>
+        <v>384.1156005859375</v>
       </c>
       <c r="F7">
-        <v>415.545654296875</v>
+        <v>384.1156005859375</v>
       </c>
       <c r="G7">
-        <v>353.7933349609375</v>
+        <v>538.9549255371094</v>
       </c>
       <c r="H7">
-        <v>97.70248413085938</v>
+        <v>538.9549255371094</v>
       </c>
       <c r="I7">
-        <v>99.47723388671875</v>
+        <v>538.9549255371094</v>
       </c>
       <c r="J7">
-        <v>248.736572265625</v>
+        <v>538.9549255371094</v>
       </c>
       <c r="K7">
-        <v>85.260009765625</v>
+        <v>647.10693359375</v>
       </c>
       <c r="L7">
-        <v>87.00729370117188</v>
+        <v>647.10693359375</v>
       </c>
       <c r="M7">
-        <v>85.77178955078125</v>
+        <v>647.10693359375</v>
       </c>
       <c r="N7">
-        <v>88.82644653320312</v>
+        <v>647.10693359375</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -2436,40 +2436,40 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -2478,40 +2478,40 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>139.2930099815131</v>
+        <v>217.669677734375</v>
       </c>
       <c r="D9">
-        <v>176.6782638877631</v>
+        <v>217.669677734375</v>
       </c>
       <c r="E9">
-        <v>160.5771896690131</v>
+        <v>217.669677734375</v>
       </c>
       <c r="F9">
-        <v>191.3413498252631</v>
+        <v>217.669677734375</v>
       </c>
       <c r="G9">
-        <v>99.300537109375</v>
+        <v>290.2414957682292</v>
       </c>
       <c r="H9">
-        <v>98.46832275390625</v>
+        <v>290.2414957682292</v>
       </c>
       <c r="I9">
-        <v>99.6514892578125</v>
+        <v>290.2414957682292</v>
       </c>
       <c r="J9">
-        <v>96.37054443359375</v>
+        <v>290.2414957682292</v>
       </c>
       <c r="K9">
-        <v>90.17333984375</v>
+        <v>396.148681640625</v>
       </c>
       <c r="L9">
-        <v>91.33819580078125</v>
+        <v>396.148681640625</v>
       </c>
       <c r="M9">
-        <v>90.5145263671875</v>
+        <v>279.6572777274782</v>
       </c>
       <c r="N9">
-        <v>92.55096435546875</v>
+        <v>396.148681640625</v>
       </c>
     </row>
   </sheetData>
@@ -2601,40 +2601,40 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>445.704749967903</v>
+        <v>1347.86865234375</v>
       </c>
       <c r="C4">
-        <v>445.704749967903</v>
+        <v>1347.86865234375</v>
       </c>
       <c r="D4">
-        <v>445.704749967903</v>
+        <v>1347.86865234375</v>
       </c>
       <c r="E4">
-        <v>342.3220484845998</v>
+        <v>1035.22602842289</v>
       </c>
       <c r="F4">
-        <v>237.679948559513</v>
+        <v>718.77482117279</v>
       </c>
       <c r="G4">
-        <v>213.7453217943979</v>
+        <v>646.3934226694769</v>
       </c>
       <c r="H4">
-        <v>208.2707913826852</v>
+        <v>629.8377365818112</v>
       </c>
       <c r="I4">
-        <v>207.0186104515645</v>
+        <v>626.0509799357542</v>
       </c>
       <c r="J4">
-        <v>206.7322010307843</v>
+        <v>625.1848409053011</v>
       </c>
       <c r="K4">
-        <v>206.6666910439502</v>
+        <v>624.9867302554246</v>
       </c>
       <c r="L4">
-        <v>206.6517070452978</v>
+        <v>624.9414167108151</v>
       </c>
       <c r="M4">
-        <v>206.6482797783044</v>
+        <v>624.9310522133669</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -2642,40 +2642,40 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>592.5830210745335</v>
+        <v>1489.3798828125</v>
       </c>
       <c r="C5">
-        <v>592.5830210745335</v>
+        <v>1489.3798828125</v>
       </c>
       <c r="D5">
-        <v>592.5830210745335</v>
+        <v>1489.3798828125</v>
       </c>
       <c r="E5">
-        <v>592.5830210745335</v>
+        <v>1489.3798828125</v>
       </c>
       <c r="F5">
-        <v>490.2392303395762</v>
+        <v>1232.152156687277</v>
       </c>
       <c r="G5">
-        <v>295.6663946043857</v>
+        <v>743.1187943066077</v>
       </c>
       <c r="H5">
-        <v>241.8674639191255</v>
+        <v>607.9022217255102</v>
       </c>
       <c r="I5">
-        <v>226.9921863299325</v>
+        <v>570.5151579645166</v>
       </c>
       <c r="J5">
-        <v>222.8792071212922</v>
+        <v>560.1777229150497</v>
       </c>
       <c r="K5">
-        <v>221.7419780599</v>
+        <v>557.3194464779085</v>
       </c>
       <c r="L5">
-        <v>221.427536903631</v>
+        <v>556.5291397768726</v>
       </c>
       <c r="M5">
-        <v>221.3405946647169</v>
+        <v>556.3106218359253</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -2683,40 +2683,40 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>250.7966110557318</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>250.7966110557318</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>250.7966110557318</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>250.7966110557318</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>151.6720823154902</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>119.2316011052148</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>111.9118487467763</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>110.2602464095121</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>109.8875848566507</v>
+        <v>1409.368286132812</v>
       </c>
       <c r="K6">
-        <v>109.8034988573471</v>
+        <v>1409.368286132812</v>
       </c>
       <c r="L6">
-        <v>109.7845259978594</v>
+        <v>1409.368286132812</v>
       </c>
       <c r="M6">
-        <v>109.7802450307529</v>
+        <v>852.3313844128272</v>
       </c>
     </row>
   </sheetData>
@@ -2803,40 +2803,40 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>570.0665377825499</v>
+        <v>665.9912109375</v>
       </c>
       <c r="C4">
-        <v>570.0665377825499</v>
+        <v>665.9912109375</v>
       </c>
       <c r="D4">
-        <v>570.0665377825499</v>
+        <v>665.9912109375</v>
       </c>
       <c r="E4">
-        <v>532.8882295061643</v>
+        <v>622.5569363247311</v>
       </c>
       <c r="F4">
-        <v>418.9306788451066</v>
+        <v>489.4238332040931</v>
       </c>
       <c r="G4">
-        <v>383.3882941716578</v>
+        <v>447.9007578445885</v>
       </c>
       <c r="H4">
-        <v>372.3029286039763</v>
+        <v>434.9500660414482</v>
       </c>
       <c r="I4">
-        <v>368.8454979645252</v>
+        <v>430.9108561147311</v>
       </c>
       <c r="J4">
-        <v>367.7671549406861</v>
+        <v>429.6510611107196</v>
       </c>
       <c r="K4">
-        <v>367.4308289812312</v>
+        <v>429.2581418317204</v>
       </c>
       <c r="L4">
-        <v>367.3259317931355</v>
+        <v>429.1355936716486</v>
       </c>
       <c r="M4">
-        <v>367.2932152579972</v>
+        <v>429.097371949428</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -2844,40 +2844,40 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>589.369149081409</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>589.369149081409</v>
+        <v>1269.355590820312</v>
       </c>
       <c r="D5">
-        <v>589.369149081409</v>
+        <v>1269.355590820312</v>
       </c>
       <c r="E5">
-        <v>479.553567195442</v>
+        <v>1032.83994855536</v>
       </c>
       <c r="F5">
-        <v>353.7489539087812</v>
+        <v>761.8878814590344</v>
       </c>
       <c r="G5">
-        <v>284.9545201185474</v>
+        <v>613.7216612131065</v>
       </c>
       <c r="H5">
-        <v>247.3352786863203</v>
+        <v>532.6991059795264</v>
       </c>
       <c r="I5">
-        <v>226.7637404387434</v>
+        <v>488.3930931401458</v>
       </c>
       <c r="J5">
-        <v>215.5144921881131</v>
+        <v>464.1649906313551</v>
       </c>
       <c r="K5">
-        <v>209.3630034330506</v>
+        <v>450.9162030840646</v>
       </c>
       <c r="L5">
-        <v>205.9991507505798</v>
+        <v>443.6712951755912</v>
       </c>
       <c r="M5">
-        <v>204.1596765484929</v>
+        <v>439.709522038623</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -2885,40 +2885,40 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>411.7559806331992</v>
+        <v>595.0048828125</v>
       </c>
       <c r="C6">
-        <v>411.7559806331992</v>
+        <v>595.0048828125</v>
       </c>
       <c r="D6">
-        <v>411.7559806331992</v>
+        <v>595.0048828125</v>
       </c>
       <c r="E6">
-        <v>411.7559806331992</v>
+        <v>595.0048828125</v>
       </c>
       <c r="F6">
-        <v>315.6177578461357</v>
+        <v>456.0810670727692</v>
       </c>
       <c r="G6">
-        <v>222.9506842748873</v>
+        <v>322.1732093992811</v>
       </c>
       <c r="H6">
-        <v>192.2877005629313</v>
+        <v>277.8638954163795</v>
       </c>
       <c r="I6">
-        <v>182.1415015530233</v>
+        <v>263.2022068512277</v>
       </c>
       <c r="J6">
-        <v>178.7841846227561</v>
+        <v>258.3507412730322</v>
       </c>
       <c r="K6">
-        <v>177.6732684107586</v>
+        <v>256.7454201565847</v>
       </c>
       <c r="L6">
-        <v>177.3056728409294</v>
+        <v>256.2142289432543</v>
       </c>
       <c r="M6">
-        <v>177.1840376523358</v>
+        <v>256.0384609288499</v>
       </c>
     </row>
   </sheetData>
@@ -3005,40 +3005,40 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>589.369149081409</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>589.369149081409</v>
+        <v>700</v>
       </c>
       <c r="D4">
-        <v>589.369149081409</v>
+        <v>700</v>
       </c>
       <c r="E4">
-        <v>479.553567195442</v>
+        <v>700</v>
       </c>
       <c r="F4">
-        <v>353.7489539087812</v>
+        <v>700</v>
       </c>
       <c r="G4">
-        <v>284.9545201185474</v>
+        <v>613.721661213111</v>
       </c>
       <c r="H4">
-        <v>247.3352786863203</v>
+        <v>532.6991059795311</v>
       </c>
       <c r="I4">
-        <v>226.7637404387434</v>
+        <v>488.3930931401458</v>
       </c>
       <c r="J4">
-        <v>215.5144921881131</v>
+        <v>464.1649906313551</v>
       </c>
       <c r="K4">
-        <v>209.3630034330506</v>
+        <v>450.9162030840646</v>
       </c>
       <c r="L4">
-        <v>205.9991507505798</v>
+        <v>443.6712951755912</v>
       </c>
       <c r="M4">
-        <v>204.1596765484929</v>
+        <v>439.709522038623</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -3046,40 +3046,40 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>130.0766982100905</v>
+        <v>400</v>
       </c>
       <c r="C5">
-        <v>49.97721090540296</v>
+        <v>400</v>
       </c>
       <c r="D5">
         <v>400</v>
       </c>
       <c r="E5">
-        <v>342.3220484845998</v>
+        <v>400</v>
       </c>
       <c r="F5">
-        <v>237.679948559513</v>
+        <v>177.3945111141962</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>155.0131126108831</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>188.4574265232175</v>
       </c>
       <c r="I5">
-        <v>52.83785483633011</v>
+        <v>400</v>
       </c>
       <c r="J5">
-        <v>206.7322010307843</v>
+        <v>214.9361246305918</v>
       </c>
       <c r="K5">
-        <v>206.6666910439502</v>
+        <v>400</v>
       </c>
       <c r="L5">
-        <v>206.6517070452978</v>
+        <v>400</v>
       </c>
       <c r="M5">
-        <v>206.6482797783044</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -3090,16 +3090,16 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>569.3555908203125</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>569.3555908203125</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>332.83994855536</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>61.88788145903436</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -3169,13 +3169,13 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>53.27561320544848</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>496.07421875</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -3190,7 +3190,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>154.1807556152344</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -3210,16 +3210,16 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>41.58793185651305</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>86.0993454307318</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>70.16764377057555</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>100.7020065635443</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -3228,22 +3228,22 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>4.376943252282217E-12</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>526.5191650390625</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>22.52059339720233</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -3251,40 +3251,40 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>411.7559806331992</v>
+        <v>595.0048828125</v>
       </c>
       <c r="C10">
-        <v>411.7559806331992</v>
+        <v>595.0048828125</v>
       </c>
       <c r="D10">
-        <v>411.7559806331992</v>
+        <v>595.0048828125</v>
       </c>
       <c r="E10">
-        <v>411.7559806331992</v>
+        <v>595.0048828125</v>
       </c>
       <c r="F10">
-        <v>315.6177578461357</v>
+        <v>456.0810670727692</v>
       </c>
       <c r="G10">
-        <v>222.9506842748873</v>
+        <v>322.1732093992811</v>
       </c>
       <c r="H10">
-        <v>192.2877005629313</v>
+        <v>277.8638954163795</v>
       </c>
       <c r="I10">
-        <v>182.1415015530233</v>
+        <v>263.2022068512277</v>
       </c>
       <c r="J10">
-        <v>178.7841846227561</v>
+        <v>258.3507412730322</v>
       </c>
       <c r="K10">
-        <v>177.6732684107586</v>
+        <v>256.7454201565847</v>
       </c>
       <c r="L10">
-        <v>177.3056728409294</v>
+        <v>256.2142289432543</v>
       </c>
       <c r="M10">
-        <v>177.1840376523358</v>
+        <v>256.0384609288499</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -3292,40 +3292,40 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>200.0109995901585</v>
+        <v>585.6719970703125</v>
       </c>
       <c r="C11">
-        <v>228.7402476370335</v>
+        <v>600</v>
       </c>
       <c r="D11">
-        <v>208.2751597464085</v>
+        <v>600</v>
       </c>
       <c r="E11">
-        <v>329.5866394042969</v>
+        <v>600</v>
       </c>
       <c r="F11">
-        <v>254.842529296875</v>
+        <v>600</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>492.0182800292969</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>539.6519470214844</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>40.59904337051013</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>465.6937751611434</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>462.8354987240023</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>461.8266740820191</v>
       </c>
     </row>
   </sheetData>
@@ -3412,19 +3412,19 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>234.3114281879075</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>90.02559124909301</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>720.5331359486529</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>616.6359477474388</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>428.140696719251</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -3433,19 +3433,19 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>95.17856310505157</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>372.3935027756959</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>372.275497485072</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>372.2485063162268</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>372.2423326676405</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -3453,40 +3453,40 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>-185.0882169654714</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>-222.0577958421638</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>122.1832903757999</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-222.0577958421638</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>-98.47958533129159</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>-86.05467528251457</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>-104.6211018595805</v>
       </c>
       <c r="I5">
-        <v>173.5817864787151</v>
+        <v>-222.0577958421638</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>-119.3206052058146</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>-222.0577958421638</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>-222.0577958421638</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>-222.0577958421638</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -3494,40 +3494,40 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>-296.5135733358634</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>-440.7994102746779</v>
+        <v>-205.9400714617335</v>
       </c>
       <c r="D6">
-        <v>189.708134424882</v>
+        <v>-205.9400714617335</v>
       </c>
       <c r="E6">
-        <v>184.7181532140702</v>
+        <v>-402.8906047250424</v>
       </c>
       <c r="F6">
-        <v>109.530892846189</v>
+        <v>-628.516925218623</v>
       </c>
       <c r="G6">
-        <v>-256.6489674797006</v>
+        <v>-596.2323471543926</v>
       </c>
       <c r="H6">
-        <v>-222.7665799782355</v>
+        <v>-517.518703278967</v>
       </c>
       <c r="I6">
-        <v>-109.0599231671661</v>
+        <v>-474.4752852316635</v>
       </c>
       <c r="J6">
-        <v>178.2868366523427</v>
+        <v>-450.9376144293007</v>
       </c>
       <c r="K6">
-        <v>183.7092707160164</v>
+        <v>-438.0663794778463</v>
       </c>
       <c r="L6">
-        <v>186.7119886998836</v>
+        <v>-431.027930747443</v>
       </c>
       <c r="M6">
-        <v>188.3625676954552</v>
+        <v>-427.1790568268473</v>
       </c>
     </row>
   </sheetData>
@@ -3614,40 +3614,40 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>-222.0577958421638</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>-222.0577958421638</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>-222.0577958421638</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-222.0577958421638</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-98.47958533129159</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>-86.05467528251457</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>-104.6211018595805</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-222.0577958421638</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>-119.3206052058146</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>-222.0577958421638</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>-222.0577958421638</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>-222.0577958421638</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -3655,40 +3655,40 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>-225.178988685815</v>
+        <v>-672.7870898001406</v>
       </c>
       <c r="C5">
-        <v>-257.5233249180987</v>
+        <v>-721.6878364870322</v>
       </c>
       <c r="D5">
-        <v>-234.4830531129474</v>
+        <v>-377.4467502690685</v>
       </c>
       <c r="E5">
-        <v>-371.0595232136811</v>
+        <v>-721.6878364870322</v>
       </c>
       <c r="F5">
-        <v>-286.9101356365059</v>
+        <v>-598.10962597616</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>-495.7665306976077</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>-553.9983089002916</v>
       </c>
       <c r="I5">
-        <v>173.5817864787151</v>
+        <v>-255.8652986577484</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>-507.1116048921884</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>-607.4686609077658</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>-222.0577958421638</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>-606.6285957463031</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -3696,40 +3696,40 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>-343.3346404580387</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>-537.7328967845708</v>
+        <v>-205.9400714617324</v>
       </c>
       <c r="D6">
-        <v>110.7110837871621</v>
+        <v>-205.9400714617317</v>
       </c>
       <c r="E6">
-        <v>71.34450854914456</v>
+        <v>-402.8906047250424</v>
       </c>
       <c r="F6">
-        <v>109.530892846189</v>
+        <v>-628.516925218623</v>
       </c>
       <c r="G6">
-        <v>-256.6489674797006</v>
+        <v>-596.2323471543926</v>
       </c>
       <c r="H6">
-        <v>-222.7665799782355</v>
+        <v>-517.5187032789706</v>
       </c>
       <c r="I6">
-        <v>-109.0599231671661</v>
+        <v>-474.4752852316635</v>
       </c>
       <c r="J6">
-        <v>178.2868366523427</v>
+        <v>-889.3789341439158</v>
       </c>
       <c r="K6">
-        <v>183.7092707160164</v>
+        <v>-937.6964201227147</v>
       </c>
       <c r="L6">
-        <v>186.7119886998836</v>
+        <v>-930.6579713923114</v>
       </c>
       <c r="M6">
-        <v>188.3625676954552</v>
+        <v>-445.9323318174986</v>
       </c>
     </row>
   </sheetData>
@@ -3816,19 +3816,19 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>234.3114281879075</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>90.02559124909301</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>720.5331359486529</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>616.6359477474388</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>428.140696719251</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -3837,19 +3837,19 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>95.17856310505157</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>372.3935027756959</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>372.275497485072</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>372.2485063162268</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>372.2423326676405</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -3857,40 +3857,40 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>-296.5135733358634</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>-440.7994102746779</v>
+        <v>-680.0519997666265</v>
       </c>
       <c r="D5">
-        <v>189.708134424882</v>
+        <v>-680.0519997666265</v>
       </c>
       <c r="E5">
-        <v>184.7181532140702</v>
+        <v>-680.0519997666265</v>
       </c>
       <c r="F5">
-        <v>109.530892846189</v>
+        <v>-680.0519997666265</v>
       </c>
       <c r="G5">
-        <v>-256.6489674797006</v>
+        <v>-596.2323471543889</v>
       </c>
       <c r="H5">
-        <v>-222.7665799782355</v>
+        <v>-517.5187032789631</v>
       </c>
       <c r="I5">
-        <v>-109.0599231671661</v>
+        <v>-474.4752852316635</v>
       </c>
       <c r="J5">
-        <v>178.2868366523427</v>
+        <v>-450.9376144293007</v>
       </c>
       <c r="K5">
-        <v>183.7092707160164</v>
+        <v>-438.0663794778463</v>
       </c>
       <c r="L5">
-        <v>186.7119886998836</v>
+        <v>-431.027930747443</v>
       </c>
       <c r="M5">
-        <v>188.3625676954552</v>
+        <v>-427.1790568268473</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -3898,40 +3898,40 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>-229.2570530171735</v>
+        <v>-495.4705229725076</v>
       </c>
       <c r="C6">
-        <v>-373.542889955988</v>
+        <v>-495.4705229725076</v>
       </c>
       <c r="D6">
-        <v>256.9646547435719</v>
+        <v>-495.4705229725076</v>
       </c>
       <c r="E6">
-        <v>153.0674665423578</v>
+        <v>-495.4705229725076</v>
       </c>
       <c r="F6">
-        <v>72.8078016849405</v>
+        <v>-379.7863367982044</v>
       </c>
       <c r="G6">
-        <v>-251.005243285129</v>
+        <v>-268.2790228447508</v>
       </c>
       <c r="H6">
-        <v>-216.483843579632</v>
+        <v>-231.3819156010453</v>
       </c>
       <c r="I6">
-        <v>-109.8823545518177</v>
+        <v>-219.1728821781633</v>
       </c>
       <c r="J6">
-        <v>171.1123633940438</v>
+        <v>-215.132985604795</v>
       </c>
       <c r="K6">
-        <v>172.2450642628054</v>
+        <v>-213.7962078470304</v>
       </c>
       <c r="L6">
-        <v>172.631924326288</v>
+        <v>-213.3538760345196</v>
       </c>
       <c r="M6">
-        <v>172.7626915900129</v>
+        <v>-213.2075110675514</v>
       </c>
     </row>
   </sheetData>

</xml_diff>